<commit_message>
quite a few updates
Currently grappling with modals and offcanvas
</commit_message>
<xml_diff>
--- a/Database tables.xlsx
+++ b/Database tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27630"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob.sharepoint.com/teams/grp-AndyRobinJazz/Shared Documents/Data Access/Data Team/Data Documentation/EXPLORE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A333181D-B86E-4369-B6E9-DD1E3B70DDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EC99312-D8C1-49F9-806F-4952A3394EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5321,15 +5321,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="C300" sqref="C300:C336"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
     <col min="11" max="11" width="78.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16969,6 +16971,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="cdd28b36-9559-4f02-b334-18686e08c090">
@@ -16977,15 +16988,6 @@
     <TaxCatchAll xmlns="edb9d0e4-5370-4cfb-9e4e-bdf6de379f60" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17249,11 +17251,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B63753ED-2BDE-41D8-AA6D-C8D4B1838EF9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECFE642C-065B-42D7-988C-837700AA9EA7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECFE642C-065B-42D7-988C-837700AA9EA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B63753ED-2BDE-41D8-AA6D-C8D4B1838EF9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
I hope search works now
</commit_message>
<xml_diff>
--- a/Database tables.xlsx
+++ b/Database tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob.sharepoint.com/teams/grp-AndyRobinJazz/Shared Documents/Data Access/Data Team/Data Documentation/EXPLORE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/bq21582_bristol_ac_uk/Documents/Programs/web app/web-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51645ED2-F023-4EEF-BC63-C5C7AD02F1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{51645ED2-F023-4EEF-BC63-C5C7AD02F1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{617505B1-A2F5-4B72-A910-274E4225D87E}"/>
   <bookViews>
-    <workbookView xWindow="15075" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3386" uniqueCount="1636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3390" uniqueCount="1636">
   <si>
     <t>source</t>
   </si>
@@ -4985,7 +4985,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5249,7 +5249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5535,9 +5535,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -5587,9 +5584,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5627,7 +5624,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5733,7 +5730,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5875,7 +5872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5893,23 +5890,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E114" workbookViewId="0">
-      <selection activeCell="I117" sqref="I117"/>
+    <sheetView tabSelected="1" topLeftCell="B370" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F374" sqref="F374"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.84375" customWidth="1"/>
+    <col min="5" max="5" width="36.3046875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="23.3046875" style="50" customWidth="1"/>
     <col min="8" max="8" width="17" style="50" customWidth="1"/>
-    <col min="11" max="11" width="78.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="54.28515625" customWidth="1"/>
+    <col min="11" max="11" width="78.84375" customWidth="1"/>
+    <col min="12" max="12" width="19.3828125" customWidth="1"/>
+    <col min="13" max="13" width="54.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5950,7 +5947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -5964,7 +5961,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="86.45">
+    <row r="3" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -5993,7 +5990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="86.45">
+    <row r="4" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -6022,7 +6019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="86.45">
+    <row r="5" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -6051,7 +6048,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="86.45">
+    <row r="6" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -6080,7 +6077,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="45.75">
+    <row r="7" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -6107,7 +6104,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="45.75">
+    <row r="8" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -6134,7 +6131,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="72">
+    <row r="9" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -6163,7 +6160,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="72">
+    <row r="10" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -6192,7 +6189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="72">
+    <row r="11" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -6221,7 +6218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="72">
+    <row r="12" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -6250,7 +6247,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="86.45">
+    <row r="13" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -6279,7 +6276,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="72">
+    <row r="14" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -6308,7 +6305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="72">
+    <row r="15" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -6337,7 +6334,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="72">
+    <row r="16" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -6366,7 +6363,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="72">
+    <row r="17" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -6393,7 +6390,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="72">
+    <row r="18" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -6420,7 +6417,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="72">
+    <row r="19" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -6447,7 +6444,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="72">
+    <row r="20" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -6474,7 +6471,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="167.25">
+    <row r="21" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -6493,10 +6490,10 @@
       <c r="F21" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G21" s="101" t="s">
+      <c r="G21" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="101" t="s">
+      <c r="H21" s="100" t="s">
         <v>44</v>
       </c>
       <c r="I21" s="2">
@@ -6512,7 +6509,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="167.25">
+    <row r="22" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
@@ -6531,10 +6528,10 @@
       <c r="F22" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="101" t="s">
+      <c r="G22" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="101" t="s">
+      <c r="H22" s="100" t="s">
         <v>20</v>
       </c>
       <c r="I22" s="2">
@@ -6550,7 +6547,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="137.25">
+    <row r="23" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>72</v>
       </c>
@@ -6569,10 +6566,10 @@
       <c r="F23" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G23" s="101" t="s">
+      <c r="G23" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="101" t="s">
+      <c r="H23" s="100" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="2">
@@ -6588,7 +6585,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="144">
+    <row r="24" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -6607,10 +6604,10 @@
       <c r="F24" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="G24" s="101" t="s">
+      <c r="G24" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="101" t="s">
+      <c r="H24" s="100" t="s">
         <v>20</v>
       </c>
       <c r="I24" s="2">
@@ -6626,7 +6623,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="72">
+    <row r="25" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>72</v>
       </c>
@@ -6645,10 +6642,10 @@
       <c r="F25" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="101" t="s">
+      <c r="G25" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="101" t="s">
+      <c r="H25" s="100" t="s">
         <v>99</v>
       </c>
       <c r="I25" s="2">
@@ -6664,7 +6661,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="144">
+    <row r="26" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>72</v>
       </c>
@@ -6683,10 +6680,10 @@
       <c r="F26" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="101" t="s">
+      <c r="G26" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="H26" s="101" t="s">
+      <c r="H26" s="100" t="s">
         <v>107</v>
       </c>
       <c r="I26" s="2">
@@ -6702,7 +6699,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="187.15">
+    <row r="27" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>72</v>
       </c>
@@ -6721,10 +6718,10 @@
       <c r="F27" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G27" s="101" t="s">
+      <c r="G27" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="101" t="s">
+      <c r="H27" s="100" t="s">
         <v>115</v>
       </c>
       <c r="I27" s="2">
@@ -6740,7 +6737,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="86.45">
+    <row r="28" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>72</v>
       </c>
@@ -6759,10 +6756,10 @@
       <c r="F28" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="101" t="s">
+      <c r="G28" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="H28" s="101" t="s">
+      <c r="H28" s="100" t="s">
         <v>115</v>
       </c>
       <c r="I28" s="2">
@@ -6778,7 +6775,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="86.45">
+    <row r="29" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>72</v>
       </c>
@@ -6797,10 +6794,10 @@
       <c r="F29" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G29" s="101" t="s">
+      <c r="G29" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="H29" s="101" t="s">
+      <c r="H29" s="100" t="s">
         <v>115</v>
       </c>
       <c r="I29" s="2">
@@ -6816,7 +6813,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="57.6">
+    <row r="30" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>72</v>
       </c>
@@ -6835,10 +6832,10 @@
       <c r="F30" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G30" s="101" t="s">
+      <c r="G30" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="H30" s="101" t="s">
+      <c r="H30" s="100" t="s">
         <v>133</v>
       </c>
       <c r="I30" s="2">
@@ -6854,7 +6851,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="57.6">
+    <row r="31" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
@@ -6873,10 +6870,10 @@
       <c r="F31" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G31" s="101" t="s">
+      <c r="G31" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="H31" s="101" t="s">
+      <c r="H31" s="100" t="s">
         <v>133</v>
       </c>
       <c r="I31" s="2">
@@ -6892,7 +6889,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="72">
+    <row r="32" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
@@ -6911,10 +6908,10 @@
       <c r="F32" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G32" s="101" t="s">
+      <c r="G32" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="H32" s="101" t="s">
+      <c r="H32" s="100" t="s">
         <v>115</v>
       </c>
       <c r="I32" s="2">
@@ -6930,7 +6927,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="43.15">
+    <row r="33" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>72</v>
       </c>
@@ -6949,10 +6946,10 @@
       <c r="F33" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="101" t="s">
+      <c r="G33" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="H33" s="101" t="s">
+      <c r="H33" s="100" t="s">
         <v>115</v>
       </c>
       <c r="I33" s="2">
@@ -6968,7 +6965,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="72">
+    <row r="34" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>72</v>
       </c>
@@ -6987,10 +6984,10 @@
       <c r="F34" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G34" s="101" t="s">
+      <c r="G34" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="H34" s="101" t="s">
+      <c r="H34" s="100" t="s">
         <v>115</v>
       </c>
       <c r="I34" s="2">
@@ -7006,7 +7003,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="57.6">
+    <row r="35" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>72</v>
       </c>
@@ -7025,10 +7022,10 @@
       <c r="F35" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G35" s="101" t="s">
+      <c r="G35" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="H35" s="101" t="s">
+      <c r="H35" s="100" t="s">
         <v>115</v>
       </c>
       <c r="I35" s="2">
@@ -7044,7 +7041,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="57.6">
+    <row r="36" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
@@ -7063,10 +7060,10 @@
       <c r="F36" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G36" s="101" t="s">
+      <c r="G36" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="H36" s="101" t="s">
+      <c r="H36" s="100" t="s">
         <v>133</v>
       </c>
       <c r="I36" s="2">
@@ -7082,7 +7079,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="129.6">
+    <row r="37" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -7101,10 +7098,10 @@
       <c r="F37" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="101" t="s">
+      <c r="G37" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="H37" s="101" t="s">
+      <c r="H37" s="100" t="s">
         <v>107</v>
       </c>
       <c r="I37" s="2">
@@ -7120,7 +7117,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="57.6">
+    <row r="38" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>72</v>
       </c>
@@ -7139,10 +7136,10 @@
       <c r="F38" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G38" s="101" t="s">
+      <c r="G38" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="H38" s="101" t="s">
+      <c r="H38" s="100" t="s">
         <v>107</v>
       </c>
       <c r="I38" s="2">
@@ -7158,7 +7155,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="129.6">
+    <row r="39" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>72</v>
       </c>
@@ -7177,10 +7174,10 @@
       <c r="F39" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="G39" s="101" t="s">
+      <c r="G39" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="H39" s="101" t="s">
+      <c r="H39" s="100" t="s">
         <v>179</v>
       </c>
       <c r="I39" s="2">
@@ -7196,7 +7193,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="57.6">
+    <row r="40" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>72</v>
       </c>
@@ -7215,10 +7212,10 @@
       <c r="F40" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="G40" s="101" t="s">
+      <c r="G40" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="H40" s="101" t="s">
+      <c r="H40" s="100" t="s">
         <v>179</v>
       </c>
       <c r="I40" s="2">
@@ -7234,7 +7231,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="57.6">
+    <row r="41" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>
@@ -7253,10 +7250,10 @@
       <c r="F41" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="G41" s="101" t="s">
+      <c r="G41" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="H41" s="101" t="s">
+      <c r="H41" s="100" t="s">
         <v>179</v>
       </c>
       <c r="I41" s="2">
@@ -7272,7 +7269,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="216">
+    <row r="42" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>72</v>
       </c>
@@ -7291,10 +7288,10 @@
       <c r="F42" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="G42" s="101" t="s">
+      <c r="G42" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="H42" s="101" t="s">
+      <c r="H42" s="100" t="s">
         <v>179</v>
       </c>
       <c r="I42" s="2">
@@ -7310,7 +7307,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="86.45">
+    <row r="43" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
@@ -7329,10 +7326,10 @@
       <c r="F43" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="G43" s="101" t="s">
+      <c r="G43" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="H43" s="101" t="s">
+      <c r="H43" s="100" t="s">
         <v>179</v>
       </c>
       <c r="I43" s="2">
@@ -7348,7 +7345,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="201.6">
+    <row r="44" spans="1:12" ht="204" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -7367,10 +7364,10 @@
       <c r="F44" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="G44" s="101" t="s">
+      <c r="G44" s="100" t="s">
         <v>204</v>
       </c>
-      <c r="H44" s="101" t="s">
+      <c r="H44" s="100" t="s">
         <v>205</v>
       </c>
       <c r="I44" s="2">
@@ -7386,7 +7383,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="43.15">
+    <row r="45" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
@@ -7405,10 +7402,10 @@
       <c r="F45" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="G45" s="101" t="s">
+      <c r="G45" s="100" t="s">
         <v>204</v>
       </c>
-      <c r="H45" s="101" t="s">
+      <c r="H45" s="100" t="s">
         <v>205</v>
       </c>
       <c r="I45" s="2">
@@ -7424,7 +7421,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="72">
+    <row r="46" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
@@ -7443,10 +7440,10 @@
       <c r="F46" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="G46" s="101" t="s">
+      <c r="G46" s="100" t="s">
         <v>204</v>
       </c>
-      <c r="H46" s="101" t="s">
+      <c r="H46" s="100" t="s">
         <v>205</v>
       </c>
       <c r="I46" s="2">
@@ -7462,7 +7459,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="158.44999999999999">
+    <row r="47" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>72</v>
       </c>
@@ -7481,10 +7478,10 @@
       <c r="F47" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="G47" s="101" t="s">
+      <c r="G47" s="100" t="s">
         <v>222</v>
       </c>
-      <c r="H47" s="101" t="s">
+      <c r="H47" s="100" t="s">
         <v>223</v>
       </c>
       <c r="I47" s="2">
@@ -7500,7 +7497,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="100.9">
+    <row r="48" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>72</v>
       </c>
@@ -7519,10 +7516,10 @@
       <c r="F48" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="G48" s="101" t="s">
+      <c r="G48" s="100" t="s">
         <v>222</v>
       </c>
-      <c r="H48" s="101" t="s">
+      <c r="H48" s="100" t="s">
         <v>223</v>
       </c>
       <c r="I48" s="2">
@@ -7538,7 +7535,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="72">
+    <row r="49" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>72</v>
       </c>
@@ -7557,10 +7554,10 @@
       <c r="F49" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="G49" s="101" t="s">
+      <c r="G49" s="100" t="s">
         <v>222</v>
       </c>
-      <c r="H49" s="101" t="s">
+      <c r="H49" s="100" t="s">
         <v>223</v>
       </c>
       <c r="I49" s="2">
@@ -7576,7 +7573,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="115.15">
+    <row r="50" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>72</v>
       </c>
@@ -7595,10 +7592,10 @@
       <c r="F50" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="G50" s="101" t="s">
+      <c r="G50" s="100" t="s">
         <v>240</v>
       </c>
-      <c r="H50" s="101" t="s">
+      <c r="H50" s="100" t="s">
         <v>241</v>
       </c>
       <c r="I50" s="2">
@@ -7614,7 +7611,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="72">
+    <row r="51" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>72</v>
       </c>
@@ -7633,10 +7630,10 @@
       <c r="F51" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="G51" s="101" t="s">
+      <c r="G51" s="100" t="s">
         <v>240</v>
       </c>
-      <c r="H51" s="101" t="s">
+      <c r="H51" s="100" t="s">
         <v>241</v>
       </c>
       <c r="I51" s="2">
@@ -7652,7 +7649,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="115.15">
+    <row r="52" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>72</v>
       </c>
@@ -7671,10 +7668,10 @@
       <c r="F52" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="G52" s="101" t="s">
+      <c r="G52" s="100" t="s">
         <v>254</v>
       </c>
-      <c r="H52" s="101" t="s">
+      <c r="H52" s="100" t="s">
         <v>255</v>
       </c>
       <c r="I52" s="2">
@@ -7690,7 +7687,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="57.6">
+    <row r="53" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>72</v>
       </c>
@@ -7709,10 +7706,10 @@
       <c r="F53" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="G53" s="101" t="s">
+      <c r="G53" s="100" t="s">
         <v>254</v>
       </c>
-      <c r="H53" s="101" t="s">
+      <c r="H53" s="100" t="s">
         <v>255</v>
       </c>
       <c r="I53" s="2">
@@ -7728,7 +7725,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="187.15">
+    <row r="54" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>72</v>
       </c>
@@ -7747,10 +7744,10 @@
       <c r="F54" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="G54" s="101" t="s">
+      <c r="G54" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="H54" s="101" t="s">
+      <c r="H54" s="100" t="s">
         <v>267</v>
       </c>
       <c r="I54" s="2">
@@ -7766,7 +7763,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="129.6">
+    <row r="55" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>72</v>
       </c>
@@ -7785,10 +7782,10 @@
       <c r="F55" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="G55" s="101" t="s">
+      <c r="G55" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="H55" s="101" t="s">
+      <c r="H55" s="100" t="s">
         <v>267</v>
       </c>
       <c r="I55" s="2">
@@ -7804,7 +7801,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="187.15">
+    <row r="56" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>72</v>
       </c>
@@ -7823,10 +7820,10 @@
       <c r="F56" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="G56" s="101" t="s">
+      <c r="G56" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="H56" s="101" t="s">
+      <c r="H56" s="100" t="s">
         <v>267</v>
       </c>
       <c r="I56" s="2">
@@ -7842,7 +7839,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="43.15">
+    <row r="57" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>72</v>
       </c>
@@ -7861,10 +7858,10 @@
       <c r="F57" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="G57" s="101" t="s">
+      <c r="G57" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="H57" s="101" t="s">
+      <c r="H57" s="100" t="s">
         <v>267</v>
       </c>
       <c r="I57" s="2">
@@ -7880,7 +7877,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="43.15">
+    <row r="58" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>72</v>
       </c>
@@ -7893,10 +7890,10 @@
       <c r="F58" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="G58" s="101" t="s">
+      <c r="G58" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="H58" s="101" t="s">
+      <c r="H58" s="100" t="s">
         <v>267</v>
       </c>
       <c r="I58" s="2">
@@ -7912,7 +7909,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="216">
+    <row r="59" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>72</v>
       </c>
@@ -7931,10 +7928,10 @@
       <c r="F59" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="G59" s="101" t="s">
+      <c r="G59" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="H59" s="101" t="s">
+      <c r="H59" s="100" t="s">
         <v>267</v>
       </c>
       <c r="I59" s="2">
@@ -7950,7 +7947,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="158.44999999999999">
+    <row r="60" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>72</v>
       </c>
@@ -7969,10 +7966,10 @@
       <c r="F60" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="G60" s="101" t="s">
+      <c r="G60" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="H60" s="101" t="s">
+      <c r="H60" s="100" t="s">
         <v>295</v>
       </c>
       <c r="I60" s="2">
@@ -7988,7 +7985,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="57.6">
+    <row r="61" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>72</v>
       </c>
@@ -8007,10 +8004,10 @@
       <c r="F61" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="G61" s="101" t="s">
+      <c r="G61" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="H61" s="101" t="s">
+      <c r="H61" s="100" t="s">
         <v>295</v>
       </c>
       <c r="I61" s="2">
@@ -8026,7 +8023,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="201.6">
+    <row r="62" spans="1:12" ht="204" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>72</v>
       </c>
@@ -8045,10 +8042,10 @@
       <c r="F62" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G62" s="101" t="s">
+      <c r="G62" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H62" s="101" t="s">
+      <c r="H62" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I62" s="2">
@@ -8064,7 +8061,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="72">
+    <row r="63" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -8083,10 +8080,10 @@
       <c r="F63" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G63" s="101" t="s">
+      <c r="G63" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H63" s="101" t="s">
+      <c r="H63" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I63" s="2">
@@ -8102,7 +8099,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="86.45">
+    <row r="64" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>72</v>
       </c>
@@ -8121,10 +8118,10 @@
       <c r="F64" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G64" s="101" t="s">
+      <c r="G64" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H64" s="101" t="s">
+      <c r="H64" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I64" s="2">
@@ -8140,7 +8137,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="57.6">
+    <row r="65" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>72</v>
       </c>
@@ -8159,10 +8156,10 @@
       <c r="F65" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G65" s="101" t="s">
+      <c r="G65" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H65" s="101" t="s">
+      <c r="H65" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I65" s="2">
@@ -8178,7 +8175,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="57.6">
+    <row r="66" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>72</v>
       </c>
@@ -8197,10 +8194,10 @@
       <c r="F66" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G66" s="101" t="s">
+      <c r="G66" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H66" s="101" t="s">
+      <c r="H66" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I66" s="2">
@@ -8216,7 +8213,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="57.6">
+    <row r="67" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -8235,10 +8232,10 @@
       <c r="F67" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G67" s="101" t="s">
+      <c r="G67" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H67" s="101" t="s">
+      <c r="H67" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I67" s="2">
@@ -8254,7 +8251,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="72">
+    <row r="68" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
@@ -8273,10 +8270,10 @@
       <c r="F68" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G68" s="101" t="s">
+      <c r="G68" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H68" s="101" t="s">
+      <c r="H68" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I68" s="2">
@@ -8292,7 +8289,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="57.6">
+    <row r="69" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>72</v>
       </c>
@@ -8311,10 +8308,10 @@
       <c r="F69" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G69" s="101" t="s">
+      <c r="G69" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H69" s="101" t="s">
+      <c r="H69" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I69" s="2">
@@ -8330,7 +8327,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="57.6">
+    <row r="70" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>72</v>
       </c>
@@ -8349,10 +8346,10 @@
       <c r="F70" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G70" s="101" t="s">
+      <c r="G70" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="H70" s="101" t="s">
+      <c r="H70" s="100" t="s">
         <v>308</v>
       </c>
       <c r="I70" s="2">
@@ -8368,7 +8365,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="100.9">
+    <row r="71" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>72</v>
       </c>
@@ -8387,10 +8384,10 @@
       <c r="F71" s="21" t="s">
         <v>349</v>
       </c>
-      <c r="G71" s="101" t="s">
+      <c r="G71" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="H71" s="101" t="s">
+      <c r="H71" s="100" t="s">
         <v>99</v>
       </c>
       <c r="I71" s="2">
@@ -8406,7 +8403,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="57.6">
+    <row r="72" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
         <v>351</v>
       </c>
@@ -8435,7 +8432,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="43.15">
+    <row r="73" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>351</v>
       </c>
@@ -8462,7 +8459,7 @@
       </c>
       <c r="K73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="43.15">
+    <row r="74" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>351</v>
       </c>
@@ -8489,7 +8486,7 @@
       </c>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="86.45">
+    <row r="75" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>351</v>
       </c>
@@ -8518,7 +8515,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="86.45">
+    <row r="76" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>351</v>
       </c>
@@ -8547,7 +8544,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="72">
+    <row r="77" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>351</v>
       </c>
@@ -8576,7 +8573,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="72">
+    <row r="78" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>351</v>
       </c>
@@ -8605,7 +8602,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="43.15">
+    <row r="79" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>351</v>
       </c>
@@ -8634,7 +8631,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="43.15">
+    <row r="80" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>351</v>
       </c>
@@ -8663,7 +8660,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="57.6">
+    <row r="81" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>351</v>
       </c>
@@ -8692,7 +8689,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="72">
+    <row r="82" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>351</v>
       </c>
@@ -8721,7 +8718,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="187.15">
+    <row r="83" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>351</v>
       </c>
@@ -8748,7 +8745,7 @@
       </c>
       <c r="K83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="43.15">
+    <row r="84" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>351</v>
       </c>
@@ -8777,7 +8774,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="57.6">
+    <row r="85" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>351</v>
       </c>
@@ -8806,7 +8803,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="57.6">
+    <row r="86" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>351</v>
       </c>
@@ -8835,7 +8832,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="57.6">
+    <row r="87" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
         <v>351</v>
       </c>
@@ -8864,7 +8861,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="288">
+    <row r="88" spans="1:12" ht="291.45" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
         <v>412</v>
       </c>
@@ -8902,7 +8899,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="288">
+    <row r="89" spans="1:12" ht="291.45" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>412</v>
       </c>
@@ -8940,7 +8937,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="259.14999999999998">
+    <row r="90" spans="1:12" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
         <v>412</v>
       </c>
@@ -8978,7 +8975,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="259.14999999999998">
+    <row r="91" spans="1:12" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
         <v>412</v>
       </c>
@@ -9016,7 +9013,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="259.14999999999998">
+    <row r="92" spans="1:12" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A92" s="4" t="s">
         <v>412</v>
       </c>
@@ -9054,7 +9051,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="230.45">
+    <row r="93" spans="1:12" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="s">
         <v>412</v>
       </c>
@@ -9092,7 +9089,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="216">
+    <row r="94" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
         <v>412</v>
       </c>
@@ -9130,7 +9127,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="144">
+    <row r="95" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
         <v>412</v>
       </c>
@@ -9168,7 +9165,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="158.44999999999999">
+    <row r="96" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A96" s="4" t="s">
         <v>412</v>
       </c>
@@ -9206,7 +9203,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="144">
+    <row r="97" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A97" s="4" t="s">
         <v>412</v>
       </c>
@@ -9238,7 +9235,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="144">
+    <row r="98" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="s">
         <v>412</v>
       </c>
@@ -9270,7 +9267,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="86.45">
+    <row r="99" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="s">
         <v>412</v>
       </c>
@@ -9302,7 +9299,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="86.45">
+    <row r="100" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A100" s="4" t="s">
         <v>412</v>
       </c>
@@ -9334,7 +9331,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="86.45">
+    <row r="101" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A101" s="4" t="s">
         <v>412</v>
       </c>
@@ -9366,7 +9363,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="100.9">
+    <row r="102" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A102" s="4" t="s">
         <v>412</v>
       </c>
@@ -9398,7 +9395,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="86.45">
+    <row r="103" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="s">
         <v>412</v>
       </c>
@@ -9430,7 +9427,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="100.9">
+    <row r="104" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A104" s="4" t="s">
         <v>412</v>
       </c>
@@ -9462,7 +9459,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="100.9">
+    <row r="105" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A105" s="4" t="s">
         <v>412</v>
       </c>
@@ -9494,7 +9491,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A106" s="35" t="s">
         <v>482</v>
       </c>
@@ -9520,7 +9517,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="72">
+    <row r="107" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A107" s="5" t="s">
         <v>482</v>
       </c>
@@ -9549,7 +9546,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="72">
+    <row r="108" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A108" s="5" t="s">
         <v>482</v>
       </c>
@@ -9578,7 +9575,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="72">
+    <row r="109" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A109" s="5" t="s">
         <v>482</v>
       </c>
@@ -9607,7 +9604,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="43.15">
+    <row r="110" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A110" s="5" t="s">
         <v>482</v>
       </c>
@@ -9636,7 +9633,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="43.15">
+    <row r="111" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A111" s="5" t="s">
         <v>482</v>
       </c>
@@ -9665,7 +9662,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="43.15">
+    <row r="112" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A112" s="5" t="s">
         <v>482</v>
       </c>
@@ -9694,7 +9691,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="72">
+    <row r="113" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A113" s="5" t="s">
         <v>482</v>
       </c>
@@ -9723,7 +9720,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="57.6">
+    <row r="114" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A114" s="5" t="s">
         <v>482</v>
       </c>
@@ -9752,7 +9749,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="100.9">
+    <row r="115" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A115" s="6" t="s">
         <v>521</v>
       </c>
@@ -9781,7 +9778,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="172.9">
+    <row r="116" spans="1:11" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A116" s="6" t="s">
         <v>521</v>
       </c>
@@ -9808,7 +9805,7 @@
       </c>
       <c r="K116" s="6"/>
     </row>
-    <row r="117" spans="1:11" ht="91.5">
+    <row r="117" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A117" s="6" t="s">
         <v>521</v>
       </c>
@@ -9818,7 +9815,7 @@
       <c r="E117" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="F117" s="107" t="s">
+      <c r="F117" s="106" t="s">
         <v>532</v>
       </c>
       <c r="G117" s="25" t="s">
@@ -9835,7 +9832,7 @@
       </c>
       <c r="K117" s="6"/>
     </row>
-    <row r="118" spans="1:11" ht="57.6">
+    <row r="118" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A118" s="6" t="s">
         <v>521</v>
       </c>
@@ -9864,7 +9861,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="86.45">
+    <row r="119" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A119" s="6" t="s">
         <v>521</v>
       </c>
@@ -9893,7 +9890,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="57.6">
+    <row r="120" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A120" s="6" t="s">
         <v>521</v>
       </c>
@@ -9920,7 +9917,7 @@
       </c>
       <c r="K120" s="6"/>
     </row>
-    <row r="121" spans="1:11" ht="86.45">
+    <row r="121" spans="1:11" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A121" s="6" t="s">
         <v>521</v>
       </c>
@@ -9947,7 +9944,7 @@
       </c>
       <c r="K121" s="6"/>
     </row>
-    <row r="122" spans="1:11" ht="43.15">
+    <row r="122" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A122" s="7" t="s">
         <v>547</v>
       </c>
@@ -9974,7 +9971,7 @@
       </c>
       <c r="K122" s="7"/>
     </row>
-    <row r="123" spans="1:11" ht="72">
+    <row r="123" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A123" s="8" t="s">
         <v>553</v>
       </c>
@@ -10003,7 +10000,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="72">
+    <row r="124" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A124" s="8" t="s">
         <v>553</v>
       </c>
@@ -10032,7 +10029,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="72">
+    <row r="125" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A125" s="8" t="s">
         <v>553</v>
       </c>
@@ -10061,7 +10058,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="72">
+    <row r="126" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A126" s="8" t="s">
         <v>553</v>
       </c>
@@ -10090,7 +10087,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="72">
+    <row r="127" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A127" s="8" t="s">
         <v>553</v>
       </c>
@@ -10119,7 +10116,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="72">
+    <row r="128" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A128" s="8" t="s">
         <v>553</v>
       </c>
@@ -10148,7 +10145,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="57.6">
+    <row r="129" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A129" s="8" t="s">
         <v>553</v>
       </c>
@@ -10177,7 +10174,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="57.6">
+    <row r="130" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A130" s="8" t="s">
         <v>553</v>
       </c>
@@ -10206,7 +10203,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="57.6">
+    <row r="131" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A131" s="8" t="s">
         <v>553</v>
       </c>
@@ -10235,7 +10232,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="28.9">
+    <row r="132" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A132" s="8" t="s">
         <v>553</v>
       </c>
@@ -10260,7 +10257,7 @@
       <c r="J132" s="8"/>
       <c r="K132" s="8"/>
     </row>
-    <row r="133" spans="1:11" ht="72">
+    <row r="133" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A133" s="8" t="s">
         <v>553</v>
       </c>
@@ -10289,7 +10286,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="72">
+    <row r="134" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A134" s="8" t="s">
         <v>553</v>
       </c>
@@ -10318,7 +10315,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="43.15">
+    <row r="135" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A135" s="8" t="s">
         <v>553</v>
       </c>
@@ -10345,7 +10342,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="72">
+    <row r="136" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A136" s="8" t="s">
         <v>553</v>
       </c>
@@ -10374,7 +10371,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="72">
+    <row r="137" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A137" s="8" t="s">
         <v>553</v>
       </c>
@@ -10403,7 +10400,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="72">
+    <row r="138" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A138" s="8" t="s">
         <v>553</v>
       </c>
@@ -10432,7 +10429,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="72">
+    <row r="139" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A139" s="8" t="s">
         <v>553</v>
       </c>
@@ -10461,7 +10458,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="28.9">
+    <row r="140" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A140" s="8" t="s">
         <v>553</v>
       </c>
@@ -10488,7 +10485,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="72">
+    <row r="141" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A141" s="8" t="s">
         <v>553</v>
       </c>
@@ -10517,7 +10514,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="72">
+    <row r="142" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A142" s="8" t="s">
         <v>553</v>
       </c>
@@ -10546,7 +10543,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="72">
+    <row r="143" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A143" s="8" t="s">
         <v>553</v>
       </c>
@@ -10575,7 +10572,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="72">
+    <row r="144" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A144" s="8" t="s">
         <v>553</v>
       </c>
@@ -10604,7 +10601,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="28.9">
+    <row r="145" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A145" s="8" t="s">
         <v>553</v>
       </c>
@@ -10631,7 +10628,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="72">
+    <row r="146" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A146" s="8" t="s">
         <v>553</v>
       </c>
@@ -10660,7 +10657,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="72">
+    <row r="147" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A147" s="8" t="s">
         <v>553</v>
       </c>
@@ -10689,7 +10686,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="28.9">
+    <row r="148" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A148" s="8" t="s">
         <v>553</v>
       </c>
@@ -10716,7 +10713,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="158.44999999999999">
+    <row r="149" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A149" s="9" t="s">
         <v>602</v>
       </c>
@@ -10745,7 +10742,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="158.44999999999999">
+    <row r="150" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A150" s="10" t="s">
         <v>608</v>
       </c>
@@ -10783,7 +10780,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="144">
+    <row r="151" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A151" s="10" t="s">
         <v>608</v>
       </c>
@@ -10821,7 +10818,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="129.6">
+    <row r="152" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A152" s="10" t="s">
         <v>608</v>
       </c>
@@ -10859,7 +10856,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="158.44999999999999">
+    <row r="153" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A153" s="10" t="s">
         <v>608</v>
       </c>
@@ -10897,7 +10894,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="144">
+    <row r="154" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A154" s="10" t="s">
         <v>608</v>
       </c>
@@ -10935,7 +10932,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="129.6">
+    <row r="155" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A155" s="10" t="s">
         <v>608</v>
       </c>
@@ -10973,7 +10970,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="158.44999999999999">
+    <row r="156" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A156" s="10" t="s">
         <v>608</v>
       </c>
@@ -11011,7 +11008,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="144">
+    <row r="157" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A157" s="10" t="s">
         <v>608</v>
       </c>
@@ -11049,7 +11046,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="129.6">
+    <row r="158" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A158" s="10" t="s">
         <v>608</v>
       </c>
@@ -11087,7 +11084,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="144">
+    <row r="159" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A159" s="10" t="s">
         <v>608</v>
       </c>
@@ -11125,7 +11122,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="144">
+    <row r="160" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A160" s="10" t="s">
         <v>608</v>
       </c>
@@ -11163,7 +11160,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="100.9">
+    <row r="161" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A161" s="10" t="s">
         <v>608</v>
       </c>
@@ -11201,7 +11198,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="100.9">
+    <row r="162" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A162" s="10" t="s">
         <v>608</v>
       </c>
@@ -11237,7 +11234,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="144">
+    <row r="163" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A163" s="10" t="s">
         <v>608</v>
       </c>
@@ -11275,7 +11272,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="115.15">
+    <row r="164" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A164" s="10" t="s">
         <v>608</v>
       </c>
@@ -11311,7 +11308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="57.6">
+    <row r="165" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A165" s="10" t="s">
         <v>608</v>
       </c>
@@ -11349,7 +11346,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="57.6">
+    <row r="166" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A166" s="10" t="s">
         <v>608</v>
       </c>
@@ -11387,7 +11384,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="167" spans="1:12" ht="72">
+    <row r="167" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A167" s="10" t="s">
         <v>608</v>
       </c>
@@ -11423,7 +11420,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="168" spans="1:12" ht="158.44999999999999">
+    <row r="168" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A168" s="10" t="s">
         <v>608</v>
       </c>
@@ -11461,7 +11458,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="86.45">
+    <row r="169" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A169" s="10" t="s">
         <v>608</v>
       </c>
@@ -11499,7 +11496,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="86.45">
+    <row r="170" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A170" s="10" t="s">
         <v>608</v>
       </c>
@@ -11537,7 +11534,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="86.45">
+    <row r="171" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A171" s="10" t="s">
         <v>608</v>
       </c>
@@ -11575,7 +11572,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="115.15">
+    <row r="172" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A172" s="10" t="s">
         <v>608</v>
       </c>
@@ -11613,7 +11610,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="86.45">
+    <row r="173" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A173" s="10" t="s">
         <v>608</v>
       </c>
@@ -11651,7 +11648,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="86.45">
+    <row r="174" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A174" s="10" t="s">
         <v>608</v>
       </c>
@@ -11689,7 +11686,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="86.45">
+    <row r="175" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A175" s="10" t="s">
         <v>608</v>
       </c>
@@ -11727,7 +11724,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="72">
+    <row r="176" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A176" s="10" t="s">
         <v>608</v>
       </c>
@@ -11763,7 +11760,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="177" spans="1:12" ht="158.44999999999999">
+    <row r="177" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A177" s="10" t="s">
         <v>608</v>
       </c>
@@ -11801,7 +11798,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="86.45">
+    <row r="178" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A178" s="10" t="s">
         <v>608</v>
       </c>
@@ -11839,7 +11836,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="179" spans="1:12" ht="158.44999999999999">
+    <row r="179" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A179" s="10" t="s">
         <v>608</v>
       </c>
@@ -11877,7 +11874,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="180" spans="1:12" ht="86.45">
+    <row r="180" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A180" s="10" t="s">
         <v>608</v>
       </c>
@@ -11915,7 +11912,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="86.45">
+    <row r="181" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A181" s="10" t="s">
         <v>608</v>
       </c>
@@ -11953,7 +11950,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="182" spans="1:12" ht="100.9">
+    <row r="182" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A182" s="10" t="s">
         <v>608</v>
       </c>
@@ -11991,7 +11988,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="115.15">
+    <row r="183" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A183" s="10" t="s">
         <v>608</v>
       </c>
@@ -12029,7 +12026,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="86.45">
+    <row r="184" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A184" s="10" t="s">
         <v>608</v>
       </c>
@@ -12067,7 +12064,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="185" spans="1:12" ht="72">
+    <row r="185" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A185" s="10" t="s">
         <v>608</v>
       </c>
@@ -12105,7 +12102,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="158.44999999999999">
+    <row r="186" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A186" s="10" t="s">
         <v>608</v>
       </c>
@@ -12143,7 +12140,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="187" spans="1:12" ht="86.45">
+    <row r="187" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A187" s="10" t="s">
         <v>608</v>
       </c>
@@ -12181,7 +12178,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="72">
+    <row r="188" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A188" s="10" t="s">
         <v>608</v>
       </c>
@@ -12217,7 +12214,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="158.44999999999999">
+    <row r="189" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A189" s="10" t="s">
         <v>608</v>
       </c>
@@ -12255,7 +12252,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="190" spans="1:12" ht="144">
+    <row r="190" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A190" s="10" t="s">
         <v>608</v>
       </c>
@@ -12293,7 +12290,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="86.45">
+    <row r="191" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A191" s="10" t="s">
         <v>608</v>
       </c>
@@ -12331,7 +12328,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="192" spans="1:12" ht="86.45">
+    <row r="192" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A192" s="10" t="s">
         <v>608</v>
       </c>
@@ -12369,7 +12366,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="115.15">
+    <row r="193" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A193" s="10" t="s">
         <v>608</v>
       </c>
@@ -12407,7 +12404,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="86.45">
+    <row r="194" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A194" s="10" t="s">
         <v>608</v>
       </c>
@@ -12445,7 +12442,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="86.45">
+    <row r="195" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A195" s="10" t="s">
         <v>608</v>
       </c>
@@ -12483,7 +12480,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="86.45">
+    <row r="196" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A196" s="10" t="s">
         <v>608</v>
       </c>
@@ -12521,7 +12518,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="197" spans="1:12" ht="172.9">
+    <row r="197" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A197" s="10" t="s">
         <v>608</v>
       </c>
@@ -12559,7 +12556,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="72">
+    <row r="198" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A198" s="10" t="s">
         <v>608</v>
       </c>
@@ -12597,7 +12594,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="199" spans="1:12" ht="72">
+    <row r="199" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A199" s="10" t="s">
         <v>608</v>
       </c>
@@ -12633,7 +12630,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="200" spans="1:12" ht="158.44999999999999">
+    <row r="200" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A200" s="10" t="s">
         <v>608</v>
       </c>
@@ -12671,7 +12668,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="201" spans="1:12" ht="86.45">
+    <row r="201" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A201" s="10" t="s">
         <v>608</v>
       </c>
@@ -12707,7 +12704,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="202" spans="1:12" ht="86.45">
+    <row r="202" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A202" s="10" t="s">
         <v>608</v>
       </c>
@@ -12745,7 +12742,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="100.9">
+    <row r="203" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A203" s="10" t="s">
         <v>608</v>
       </c>
@@ -12781,7 +12778,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="115.15">
+    <row r="204" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A204" s="10" t="s">
         <v>608</v>
       </c>
@@ -12819,7 +12816,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="115.15">
+    <row r="205" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A205" s="10" t="s">
         <v>608</v>
       </c>
@@ -12857,7 +12854,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="206" spans="1:12" ht="72">
+    <row r="206" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A206" s="10" t="s">
         <v>608</v>
       </c>
@@ -12895,7 +12892,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="207" spans="1:12" ht="201.6">
+    <row r="207" spans="1:12" ht="204" x14ac:dyDescent="0.4">
       <c r="A207" s="10" t="s">
         <v>608</v>
       </c>
@@ -12933,7 +12930,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="208" spans="1:12" ht="86.45">
+    <row r="208" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A208" s="10" t="s">
         <v>608</v>
       </c>
@@ -12971,7 +12968,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="209" spans="1:12" ht="57.6">
+    <row r="209" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A209" s="10" t="s">
         <v>608</v>
       </c>
@@ -13007,7 +13004,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="210" spans="1:12" ht="158.44999999999999">
+    <row r="210" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A210" s="10" t="s">
         <v>608</v>
       </c>
@@ -13045,7 +13042,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="211" spans="1:12" ht="86.45">
+    <row r="211" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A211" s="10" t="s">
         <v>608</v>
       </c>
@@ -13083,7 +13080,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="72">
+    <row r="212" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A212" s="10" t="s">
         <v>608</v>
       </c>
@@ -13121,7 +13118,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="100.9">
+    <row r="213" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A213" s="10" t="s">
         <v>608</v>
       </c>
@@ -13159,7 +13156,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="115.15">
+    <row r="214" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A214" s="10" t="s">
         <v>608</v>
       </c>
@@ -13197,7 +13194,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="215" spans="1:12" ht="86.45">
+    <row r="215" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A215" s="10" t="s">
         <v>608</v>
       </c>
@@ -13235,7 +13232,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="216" spans="1:12" ht="86.45">
+    <row r="216" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A216" s="10" t="s">
         <v>608</v>
       </c>
@@ -13273,7 +13270,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="217" spans="1:12" ht="201.6">
+    <row r="217" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A217" s="10" t="s">
         <v>608</v>
       </c>
@@ -13311,7 +13308,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="218" spans="1:12" ht="57.6">
+    <row r="218" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A218" s="10" t="s">
         <v>608</v>
       </c>
@@ -13347,7 +13344,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="219" spans="1:12" ht="158.44999999999999">
+    <row r="219" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A219" s="10" t="s">
         <v>608</v>
       </c>
@@ -13385,7 +13382,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="220" spans="1:12" ht="86.45">
+    <row r="220" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A220" s="10" t="s">
         <v>608</v>
       </c>
@@ -13423,7 +13420,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="221" spans="1:12" ht="86.45">
+    <row r="221" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A221" s="10" t="s">
         <v>608</v>
       </c>
@@ -13461,7 +13458,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="222" spans="1:12" ht="86.45">
+    <row r="222" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A222" s="10" t="s">
         <v>608</v>
       </c>
@@ -13499,7 +13496,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="100.9">
+    <row r="223" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A223" s="10" t="s">
         <v>608</v>
       </c>
@@ -13535,7 +13532,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="115.15">
+    <row r="224" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A224" s="10" t="s">
         <v>608</v>
       </c>
@@ -13573,7 +13570,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="225" spans="1:12" ht="86.45">
+    <row r="225" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A225" s="10" t="s">
         <v>608</v>
       </c>
@@ -13611,7 +13608,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="57.6">
+    <row r="226" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A226" s="10" t="s">
         <v>608</v>
       </c>
@@ -13649,7 +13646,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="230.45">
+    <row r="227" spans="1:12" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A227" s="10" t="s">
         <v>608</v>
       </c>
@@ -13687,7 +13684,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="228" spans="1:12" ht="57.6">
+    <row r="228" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A228" s="10" t="s">
         <v>608</v>
       </c>
@@ -13723,7 +13720,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="229" spans="1:12" ht="57.6">
+    <row r="229" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A229" s="10" t="s">
         <v>608</v>
       </c>
@@ -13759,7 +13756,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="230" spans="1:12" ht="158.44999999999999">
+    <row r="230" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A230" s="10" t="s">
         <v>608</v>
       </c>
@@ -13797,7 +13794,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="231" spans="1:12" ht="86.45">
+    <row r="231" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A231" s="10" t="s">
         <v>608</v>
       </c>
@@ -13835,7 +13832,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="232" spans="1:12" ht="57.6">
+    <row r="232" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A232" s="10" t="s">
         <v>608</v>
       </c>
@@ -13873,7 +13870,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="233" spans="1:12" ht="57.6">
+    <row r="233" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A233" s="10" t="s">
         <v>608</v>
       </c>
@@ -13911,7 +13908,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="234" spans="1:12" ht="72">
+    <row r="234" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A234" s="10" t="s">
         <v>608</v>
       </c>
@@ -13947,7 +13944,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="235" spans="1:12" ht="158.44999999999999">
+    <row r="235" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A235" s="11" t="s">
         <v>967</v>
       </c>
@@ -13985,7 +13982,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="236" spans="1:12" ht="144">
+    <row r="236" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A236" s="11" t="s">
         <v>967</v>
       </c>
@@ -14023,7 +14020,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="237" spans="1:12" ht="129.6">
+    <row r="237" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A237" s="11" t="s">
         <v>967</v>
       </c>
@@ -14061,7 +14058,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="238" spans="1:12" ht="144">
+    <row r="238" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A238" s="11" t="s">
         <v>967</v>
       </c>
@@ -14099,7 +14096,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="239" spans="1:12" ht="72">
+    <row r="239" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A239" s="11" t="s">
         <v>967</v>
       </c>
@@ -14137,7 +14134,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="240" spans="1:12" ht="144">
+    <row r="240" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A240" s="11" t="s">
         <v>967</v>
       </c>
@@ -14175,7 +14172,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="241" spans="1:12" ht="100.9">
+    <row r="241" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A241" s="11" t="s">
         <v>967</v>
       </c>
@@ -14213,7 +14210,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="242" spans="1:12" ht="115.15">
+    <row r="242" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A242" s="11" t="s">
         <v>967</v>
       </c>
@@ -14251,7 +14248,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="243" spans="1:12" ht="115.15">
+    <row r="243" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A243" s="11" t="s">
         <v>967</v>
       </c>
@@ -14289,7 +14286,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="244" spans="1:12" ht="72">
+    <row r="244" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A244" s="11" t="s">
         <v>967</v>
       </c>
@@ -14327,7 +14324,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="245" spans="1:12" ht="115.15">
+    <row r="245" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A245" s="11" t="s">
         <v>967</v>
       </c>
@@ -14362,7 +14359,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="246" spans="1:12" ht="129.6">
+    <row r="246" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A246" s="11" t="s">
         <v>967</v>
       </c>
@@ -14400,7 +14397,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="247" spans="1:12" ht="115.15">
+    <row r="247" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A247" s="11" t="s">
         <v>967</v>
       </c>
@@ -14438,7 +14435,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="248" spans="1:12" ht="158.44999999999999">
+    <row r="248" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A248" s="11" t="s">
         <v>967</v>
       </c>
@@ -14476,7 +14473,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="249" spans="1:12" ht="100.9">
+    <row r="249" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A249" s="11" t="s">
         <v>967</v>
       </c>
@@ -14514,7 +14511,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="250" spans="1:12" ht="72">
+    <row r="250" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A250" s="11" t="s">
         <v>967</v>
       </c>
@@ -14552,7 +14549,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="251" spans="1:12" ht="43.15">
+    <row r="251" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A251" s="11" t="s">
         <v>967</v>
       </c>
@@ -14590,7 +14587,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="252" spans="1:12" ht="86.45">
+    <row r="252" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A252" s="11" t="s">
         <v>967</v>
       </c>
@@ -14628,7 +14625,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="253" spans="1:12" ht="86.45">
+    <row r="253" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A253" s="11" t="s">
         <v>967</v>
       </c>
@@ -14666,7 +14663,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="254" spans="1:12" ht="100.9">
+    <row r="254" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A254" s="11" t="s">
         <v>967</v>
       </c>
@@ -14704,7 +14701,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="255" spans="1:12" ht="72">
+    <row r="255" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A255" s="11" t="s">
         <v>967</v>
       </c>
@@ -14742,7 +14739,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="256" spans="1:12" ht="100.9">
+    <row r="256" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A256" s="11" t="s">
         <v>967</v>
       </c>
@@ -14780,7 +14777,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="257" spans="1:12" ht="72">
+    <row r="257" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A257" s="11" t="s">
         <v>967</v>
       </c>
@@ -14818,7 +14815,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="258" spans="1:12" ht="158.44999999999999">
+    <row r="258" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A258" s="12" t="s">
         <v>1081</v>
       </c>
@@ -14856,7 +14853,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="259" spans="1:12" ht="144">
+    <row r="259" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A259" s="12" t="s">
         <v>1081</v>
       </c>
@@ -14894,7 +14891,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="260" spans="1:12" ht="129.6">
+    <row r="260" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A260" s="12" t="s">
         <v>1081</v>
       </c>
@@ -14932,7 +14929,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="261" spans="1:12" ht="144">
+    <row r="261" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A261" s="12" t="s">
         <v>1081</v>
       </c>
@@ -14970,7 +14967,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="262" spans="1:12" ht="115.15">
+    <row r="262" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A262" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15004,7 +15001,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="263" spans="1:12" ht="187.15">
+    <row r="263" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A263" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15042,7 +15039,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="264" spans="1:12" ht="316.89999999999998">
+    <row r="264" spans="1:12" ht="320.60000000000002" x14ac:dyDescent="0.4">
       <c r="A264" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15061,10 +15058,10 @@
       <c r="F264" s="31" t="s">
         <v>1099</v>
       </c>
-      <c r="G264" s="102" t="s">
+      <c r="G264" s="101" t="s">
         <v>1100</v>
       </c>
-      <c r="H264" s="102" t="s">
+      <c r="H264" s="101" t="s">
         <v>1101</v>
       </c>
       <c r="I264" s="12">
@@ -15080,7 +15077,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="265" spans="1:12" ht="115.15">
+    <row r="265" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A265" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15099,10 +15096,10 @@
       <c r="F265" s="31" t="s">
         <v>1099</v>
       </c>
-      <c r="G265" s="102" t="s">
+      <c r="G265" s="101" t="s">
         <v>1100</v>
       </c>
-      <c r="H265" s="102" t="s">
+      <c r="H265" s="101" t="s">
         <v>1101</v>
       </c>
       <c r="I265" s="12">
@@ -15118,7 +15115,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="266" spans="1:12" ht="187.15">
+    <row r="266" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A266" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15137,10 +15134,10 @@
       <c r="F266" s="31" t="s">
         <v>1099</v>
       </c>
-      <c r="G266" s="102" t="s">
+      <c r="G266" s="101" t="s">
         <v>1100</v>
       </c>
-      <c r="H266" s="102" t="s">
+      <c r="H266" s="101" t="s">
         <v>1101</v>
       </c>
       <c r="I266" s="12">
@@ -15156,7 +15153,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="267" spans="1:12" ht="115.15">
+    <row r="267" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A267" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15175,10 +15172,10 @@
       <c r="F267" s="31" t="s">
         <v>1099</v>
       </c>
-      <c r="G267" s="102" t="s">
+      <c r="G267" s="101" t="s">
         <v>1100</v>
       </c>
-      <c r="H267" s="102" t="s">
+      <c r="H267" s="101" t="s">
         <v>1101</v>
       </c>
       <c r="I267" s="12">
@@ -15194,7 +15191,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="268" spans="1:12" ht="331.15">
+    <row r="268" spans="1:12" ht="364.3" x14ac:dyDescent="0.4">
       <c r="A268" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15213,10 +15210,10 @@
       <c r="F268" s="31" t="s">
         <v>1119</v>
       </c>
-      <c r="G268" s="102" t="s">
+      <c r="G268" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="H268" s="102" t="s">
+      <c r="H268" s="101" t="s">
         <v>1120</v>
       </c>
       <c r="I268" s="12">
@@ -15232,7 +15229,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="269" spans="1:12" ht="144">
+    <row r="269" spans="1:12" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A269" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15251,10 +15248,10 @@
       <c r="F269" s="31" t="s">
         <v>1119</v>
       </c>
-      <c r="G269" s="102" t="s">
+      <c r="G269" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="H269" s="102" t="s">
+      <c r="H269" s="101" t="s">
         <v>1120</v>
       </c>
       <c r="I269" s="12">
@@ -15270,7 +15267,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="270" spans="1:12" ht="259.14999999999998">
+    <row r="270" spans="1:12" ht="276.89999999999998" x14ac:dyDescent="0.4">
       <c r="A270" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15289,10 +15286,10 @@
       <c r="F270" s="31" t="s">
         <v>1119</v>
       </c>
-      <c r="G270" s="102" t="s">
+      <c r="G270" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="H270" s="102" t="s">
+      <c r="H270" s="101" t="s">
         <v>1120</v>
       </c>
       <c r="I270" s="12">
@@ -15308,7 +15305,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="271" spans="1:12" ht="115.15">
+    <row r="271" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A271" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15327,10 +15324,10 @@
       <c r="F271" s="12" t="s">
         <v>1119</v>
       </c>
-      <c r="G271" s="102" t="s">
+      <c r="G271" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="H271" s="102" t="s">
+      <c r="H271" s="101" t="s">
         <v>1120</v>
       </c>
       <c r="I271" s="12">
@@ -15346,7 +15343,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="272" spans="1:12" ht="331.15">
+    <row r="272" spans="1:12" ht="335.15" x14ac:dyDescent="0.4">
       <c r="A272" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15365,10 +15362,10 @@
       <c r="F272" s="12" t="s">
         <v>1137</v>
       </c>
-      <c r="G272" s="102" t="s">
+      <c r="G272" s="101" t="s">
         <v>1138</v>
       </c>
-      <c r="H272" s="102" t="s">
+      <c r="H272" s="101" t="s">
         <v>1139</v>
       </c>
       <c r="I272" s="12">
@@ -15384,7 +15381,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="273" spans="1:12" ht="115.15">
+    <row r="273" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A273" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15403,10 +15400,10 @@
       <c r="F273" s="12" t="s">
         <v>1137</v>
       </c>
-      <c r="G273" s="102" t="s">
+      <c r="G273" s="101" t="s">
         <v>1138</v>
       </c>
-      <c r="H273" s="102" t="s">
+      <c r="H273" s="101" t="s">
         <v>1139</v>
       </c>
       <c r="I273" s="12">
@@ -15422,7 +15419,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="274" spans="1:12" ht="201.6">
+    <row r="274" spans="1:12" ht="204" x14ac:dyDescent="0.4">
       <c r="A274" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15441,10 +15438,10 @@
       <c r="F274" s="12" t="s">
         <v>1137</v>
       </c>
-      <c r="G274" s="102" t="s">
+      <c r="G274" s="101" t="s">
         <v>1138</v>
       </c>
-      <c r="H274" s="102" t="s">
+      <c r="H274" s="101" t="s">
         <v>1139</v>
       </c>
       <c r="I274" s="12">
@@ -15460,7 +15457,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="275" spans="1:12" ht="100.9">
+    <row r="275" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A275" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15479,10 +15476,10 @@
       <c r="F275" s="31" t="s">
         <v>1137</v>
       </c>
-      <c r="G275" s="102" t="s">
+      <c r="G275" s="101" t="s">
         <v>1138</v>
       </c>
-      <c r="H275" s="102" t="s">
+      <c r="H275" s="101" t="s">
         <v>1139</v>
       </c>
       <c r="I275" s="12">
@@ -15498,7 +15495,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="276" spans="1:12" ht="316.89999999999998">
+    <row r="276" spans="1:12" ht="320.60000000000002" x14ac:dyDescent="0.4">
       <c r="A276" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15517,10 +15514,10 @@
       <c r="F276" s="31" t="s">
         <v>1156</v>
       </c>
-      <c r="G276" s="102" t="s">
+      <c r="G276" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="H276" s="102" t="s">
+      <c r="H276" s="101" t="s">
         <v>1157</v>
       </c>
       <c r="I276" s="12">
@@ -15536,7 +15533,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="277" spans="1:12" ht="100.9">
+    <row r="277" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A277" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15555,10 +15552,10 @@
       <c r="F277" s="31" t="s">
         <v>1156</v>
       </c>
-      <c r="G277" s="102" t="s">
+      <c r="G277" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="H277" s="102" t="s">
+      <c r="H277" s="101" t="s">
         <v>1157</v>
       </c>
       <c r="I277" s="12">
@@ -15574,7 +15571,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="278" spans="1:12" ht="216">
+    <row r="278" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A278" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15593,10 +15590,10 @@
       <c r="F278" s="31" t="s">
         <v>1156</v>
       </c>
-      <c r="G278" s="102" t="s">
+      <c r="G278" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="H278" s="102" t="s">
+      <c r="H278" s="101" t="s">
         <v>1157</v>
       </c>
       <c r="I278" s="12">
@@ -15612,7 +15609,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="279" spans="1:12" ht="115.15">
+    <row r="279" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A279" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15631,10 +15628,10 @@
       <c r="F279" s="31" t="s">
         <v>1156</v>
       </c>
-      <c r="G279" s="102" t="s">
+      <c r="G279" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="H279" s="102" t="s">
+      <c r="H279" s="101" t="s">
         <v>1157</v>
       </c>
       <c r="I279" s="12">
@@ -15650,7 +15647,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="280" spans="1:12" ht="201.6">
+    <row r="280" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A280" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15669,10 +15666,10 @@
       <c r="F280" s="31" t="s">
         <v>1174</v>
       </c>
-      <c r="G280" s="102" t="s">
+      <c r="G280" s="101" t="s">
         <v>1175</v>
       </c>
-      <c r="H280" s="102" t="s">
+      <c r="H280" s="101" t="s">
         <v>1176</v>
       </c>
       <c r="I280" s="12">
@@ -15688,7 +15685,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="281" spans="1:12" ht="57.6">
+    <row r="281" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A281" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15707,10 +15704,10 @@
       <c r="F281" s="31" t="s">
         <v>1174</v>
       </c>
-      <c r="G281" s="102" t="s">
+      <c r="G281" s="101" t="s">
         <v>1175</v>
       </c>
-      <c r="H281" s="102" t="s">
+      <c r="H281" s="101" t="s">
         <v>1176</v>
       </c>
       <c r="I281" s="12">
@@ -15726,7 +15723,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="282" spans="1:12" ht="187.15">
+    <row r="282" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A282" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15745,10 +15742,10 @@
       <c r="F282" s="31" t="s">
         <v>1174</v>
       </c>
-      <c r="G282" s="102" t="s">
+      <c r="G282" s="101" t="s">
         <v>1175</v>
       </c>
-      <c r="H282" s="102" t="s">
+      <c r="H282" s="101" t="s">
         <v>1176</v>
       </c>
       <c r="I282" s="12">
@@ -15764,7 +15761,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="283" spans="1:12" ht="244.9">
+    <row r="283" spans="1:12" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A283" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15783,10 +15780,10 @@
       <c r="F283" s="31" t="s">
         <v>1190</v>
       </c>
-      <c r="G283" s="102" t="s">
+      <c r="G283" s="101" t="s">
         <v>1191</v>
       </c>
-      <c r="H283" s="102" t="s">
+      <c r="H283" s="101" t="s">
         <v>1192</v>
       </c>
       <c r="I283" s="12">
@@ -15802,7 +15799,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="284" spans="1:12" ht="172.9">
+    <row r="284" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A284" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15821,10 +15818,10 @@
       <c r="F284" s="31" t="s">
         <v>1190</v>
       </c>
-      <c r="G284" s="102" t="s">
+      <c r="G284" s="101" t="s">
         <v>1191</v>
       </c>
-      <c r="H284" s="102" t="s">
+      <c r="H284" s="101" t="s">
         <v>1192</v>
       </c>
       <c r="I284" s="12">
@@ -15840,7 +15837,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="285" spans="1:12" ht="201.6">
+    <row r="285" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A285" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15859,10 +15856,10 @@
       <c r="F285" s="31" t="s">
         <v>1201</v>
       </c>
-      <c r="G285" s="102" t="s">
+      <c r="G285" s="101" t="s">
         <v>1202</v>
       </c>
-      <c r="H285" s="102" t="s">
+      <c r="H285" s="101" t="s">
         <v>1093</v>
       </c>
       <c r="I285" s="12">
@@ -15878,7 +15875,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="286" spans="1:12" ht="158.44999999999999">
+    <row r="286" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A286" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15897,10 +15894,10 @@
       <c r="F286" s="31" t="s">
         <v>1201</v>
       </c>
-      <c r="G286" s="102" t="s">
+      <c r="G286" s="101" t="s">
         <v>1202</v>
       </c>
-      <c r="H286" s="102" t="s">
+      <c r="H286" s="101" t="s">
         <v>1093</v>
       </c>
       <c r="I286" s="12">
@@ -15916,7 +15913,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="287" spans="1:12" ht="409.6">
+    <row r="287" spans="1:12" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A287" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15935,10 +15932,10 @@
       <c r="F287" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G287" s="102" t="s">
+      <c r="G287" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H287" s="102" t="s">
+      <c r="H287" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I287" s="12">
@@ -15954,7 +15951,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="288" spans="1:12" ht="57.6">
+    <row r="288" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A288" s="12" t="s">
         <v>1081</v>
       </c>
@@ -15973,10 +15970,10 @@
       <c r="F288" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G288" s="102" t="s">
+      <c r="G288" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H288" s="102" t="s">
+      <c r="H288" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I288" s="12">
@@ -15992,7 +15989,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="289" spans="1:12" ht="144">
+    <row r="289" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A289" s="12" t="s">
         <v>1081</v>
       </c>
@@ -16011,10 +16008,10 @@
       <c r="F289" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G289" s="102" t="s">
+      <c r="G289" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H289" s="102" t="s">
+      <c r="H289" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I289" s="12">
@@ -16030,7 +16027,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="290" spans="1:12" ht="409.6">
+    <row r="290" spans="1:12" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A290" s="12" t="s">
         <v>1081</v>
       </c>
@@ -16049,10 +16046,10 @@
       <c r="F290" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G290" s="102" t="s">
+      <c r="G290" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H290" s="102" t="s">
+      <c r="H290" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I290" s="12">
@@ -16068,7 +16065,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="291" spans="1:12" ht="100.9">
+    <row r="291" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A291" s="12" t="s">
         <v>1081</v>
       </c>
@@ -16087,10 +16084,10 @@
       <c r="F291" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G291" s="102" t="s">
+      <c r="G291" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H291" s="102" t="s">
+      <c r="H291" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I291" s="12">
@@ -16106,7 +16103,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="292" spans="1:12" ht="100.9">
+    <row r="292" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A292" s="12" t="s">
         <v>1081</v>
       </c>
@@ -16125,10 +16122,10 @@
       <c r="F292" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G292" s="102" t="s">
+      <c r="G292" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H292" s="102" t="s">
+      <c r="H292" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I292" s="12">
@@ -16144,7 +16141,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="293" spans="1:12" ht="129.6">
+    <row r="293" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A293" s="12" t="s">
         <v>1081</v>
       </c>
@@ -16163,10 +16160,10 @@
       <c r="F293" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G293" s="102" t="s">
+      <c r="G293" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H293" s="102" t="s">
+      <c r="H293" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I293" s="12">
@@ -16182,7 +16179,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="294" spans="1:12" ht="129.6">
+    <row r="294" spans="1:12" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A294" s="12" t="s">
         <v>1081</v>
       </c>
@@ -16201,10 +16198,10 @@
       <c r="F294" s="31" t="s">
         <v>1211</v>
       </c>
-      <c r="G294" s="102" t="s">
+      <c r="G294" s="101" t="s">
         <v>1212</v>
       </c>
-      <c r="H294" s="102" t="s">
+      <c r="H294" s="101" t="s">
         <v>1088</v>
       </c>
       <c r="I294" s="12">
@@ -16220,7 +16217,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="295" spans="1:12" ht="115.15">
+    <row r="295" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A295" s="13" t="s">
         <v>1241</v>
       </c>
@@ -16233,10 +16230,10 @@
       <c r="F295" s="32" t="s">
         <v>1244</v>
       </c>
-      <c r="G295" s="103" t="s">
+      <c r="G295" s="102" t="s">
         <v>622</v>
       </c>
-      <c r="H295" s="103" t="s">
+      <c r="H295" s="102" t="s">
         <v>377</v>
       </c>
       <c r="I295" s="13">
@@ -16247,7 +16244,7 @@
       </c>
       <c r="K295" s="13"/>
     </row>
-    <row r="296" spans="1:12" ht="100.9">
+    <row r="296" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A296" s="13" t="s">
         <v>1241</v>
       </c>
@@ -16260,10 +16257,10 @@
       <c r="F296" s="32" t="s">
         <v>1247</v>
       </c>
-      <c r="G296" s="103" t="s">
+      <c r="G296" s="102" t="s">
         <v>1248</v>
       </c>
-      <c r="H296" s="103" t="s">
+      <c r="H296" s="102" t="s">
         <v>1249</v>
       </c>
       <c r="I296" s="13">
@@ -16276,7 +16273,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="297" spans="1:12" ht="115.15">
+    <row r="297" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A297" s="13" t="s">
         <v>1241</v>
       </c>
@@ -16289,10 +16286,10 @@
       <c r="F297" s="32" t="s">
         <v>1253</v>
       </c>
-      <c r="G297" s="103" t="s">
+      <c r="G297" s="102" t="s">
         <v>1254</v>
       </c>
-      <c r="H297" s="103" t="s">
+      <c r="H297" s="102" t="s">
         <v>1255</v>
       </c>
       <c r="I297" s="13">
@@ -16305,7 +16302,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="298" spans="1:12" ht="129.6">
+    <row r="298" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A298" s="13" t="s">
         <v>1241</v>
       </c>
@@ -16318,10 +16315,10 @@
       <c r="F298" s="32" t="s">
         <v>1247</v>
       </c>
-      <c r="G298" s="103" t="s">
+      <c r="G298" s="102" t="s">
         <v>1248</v>
       </c>
-      <c r="H298" s="103" t="s">
+      <c r="H298" s="102" t="s">
         <v>1249</v>
       </c>
       <c r="I298" s="13">
@@ -16334,7 +16331,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="299" spans="1:12" ht="43.15">
+    <row r="299" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A299" s="13" t="s">
         <v>1241</v>
       </c>
@@ -16347,10 +16344,10 @@
       <c r="F299" s="13" t="s">
         <v>1260</v>
       </c>
-      <c r="G299" s="103" t="s">
+      <c r="G299" s="102" t="s">
         <v>1261</v>
       </c>
-      <c r="H299" s="103" t="s">
+      <c r="H299" s="102" t="s">
         <v>1262</v>
       </c>
       <c r="I299" s="13">
@@ -16361,7 +16358,7 @@
       </c>
       <c r="K299" s="13"/>
     </row>
-    <row r="300" spans="1:12" ht="158.44999999999999">
+    <row r="300" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A300" s="14" t="s">
         <v>1263</v>
       </c>
@@ -16380,10 +16377,10 @@
       <c r="F300" s="14" t="s">
         <v>605</v>
       </c>
-      <c r="G300" s="104" t="s">
+      <c r="G300" s="103" t="s">
         <v>606</v>
       </c>
-      <c r="H300" s="104" t="s">
+      <c r="H300" s="103" t="s">
         <v>529</v>
       </c>
       <c r="I300" s="14"/>
@@ -16397,7 +16394,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="301" spans="1:12" ht="57.6">
+    <row r="301" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A301" s="15" t="s">
         <v>1270</v>
       </c>
@@ -16410,10 +16407,10 @@
       <c r="F301" s="15" t="s">
         <v>1273</v>
       </c>
-      <c r="G301" s="105" t="s">
+      <c r="G301" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="H301" s="105" t="s">
+      <c r="H301" s="104" t="s">
         <v>364</v>
       </c>
       <c r="I301" s="15">
@@ -16424,7 +16421,7 @@
       </c>
       <c r="K301" s="15"/>
     </row>
-    <row r="302" spans="1:12" ht="57.6">
+    <row r="302" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A302" s="15" t="s">
         <v>1270</v>
       </c>
@@ -16453,7 +16450,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="303" spans="1:12" ht="57.6">
+    <row r="303" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A303" s="15" t="s">
         <v>1270</v>
       </c>
@@ -16482,7 +16479,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="304" spans="1:12" ht="43.15">
+    <row r="304" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A304" s="15" t="s">
         <v>1270</v>
       </c>
@@ -16509,7 +16506,7 @@
       </c>
       <c r="K304" s="15"/>
     </row>
-    <row r="305" spans="1:12" ht="57.6">
+    <row r="305" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A305" s="15" t="s">
         <v>1270</v>
       </c>
@@ -16538,7 +16535,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="306" spans="1:12" ht="57.6">
+    <row r="306" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A306" s="15" t="s">
         <v>1270</v>
       </c>
@@ -16565,7 +16562,7 @@
       </c>
       <c r="K306" s="15"/>
     </row>
-    <row r="307" spans="1:12" ht="43.15">
+    <row r="307" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A307" s="16" t="s">
         <v>1291</v>
       </c>
@@ -16594,7 +16591,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="308" spans="1:12" ht="43.15">
+    <row r="308" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A308" s="16" t="s">
         <v>1291</v>
       </c>
@@ -16623,7 +16620,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="309" spans="1:12" ht="28.9">
+    <row r="309" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A309" s="16" t="s">
         <v>1291</v>
       </c>
@@ -16652,7 +16649,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="310" spans="1:12" ht="115.15">
+    <row r="310" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A310" s="16" t="s">
         <v>1291</v>
       </c>
@@ -16681,7 +16678,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="311" spans="1:12" ht="172.9">
+    <row r="311" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A311" s="16" t="s">
         <v>1291</v>
       </c>
@@ -16710,7 +16707,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="312" spans="1:12" ht="43.15">
+    <row r="312" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A312" s="16" t="s">
         <v>1291</v>
       </c>
@@ -16739,7 +16736,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="313" spans="1:12" ht="409.6">
+    <row r="313" spans="1:12" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A313" s="16" t="s">
         <v>1291</v>
       </c>
@@ -16768,7 +16765,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="314" spans="1:12" ht="43.15">
+    <row r="314" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A314" s="17" t="s">
         <v>1315</v>
       </c>
@@ -16797,7 +16794,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="315" spans="1:12" ht="43.15">
+    <row r="315" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A315" s="17" t="s">
         <v>1315</v>
       </c>
@@ -16826,7 +16823,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="316" spans="1:12" ht="43.15">
+    <row r="316" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A316" s="17" t="s">
         <v>1315</v>
       </c>
@@ -16855,7 +16852,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="317" spans="1:12" ht="187.15">
+    <row r="317" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A317" s="18" t="s">
         <v>1328</v>
       </c>
@@ -16893,7 +16890,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="318" spans="1:12" ht="187.15">
+    <row r="318" spans="1:12" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A318" s="18" t="s">
         <v>1328</v>
       </c>
@@ -16929,7 +16926,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="319" spans="1:12" ht="216">
+    <row r="319" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A319" s="18" t="s">
         <v>1328</v>
       </c>
@@ -16965,7 +16962,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="320" spans="1:12" ht="216">
+    <row r="320" spans="1:12" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A320" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17001,7 +16998,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="321" spans="1:12" ht="201.6">
+    <row r="321" spans="1:12" ht="204" x14ac:dyDescent="0.4">
       <c r="A321" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17037,7 +17034,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="322" spans="1:12" ht="172.9">
+    <row r="322" spans="1:12" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A322" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17073,7 +17070,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="323" spans="1:12" ht="100.9">
+    <row r="323" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A323" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17109,7 +17106,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="324" spans="1:12" ht="43.15">
+    <row r="324" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A324" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17126,8 +17123,12 @@
         <v>1373</v>
       </c>
       <c r="F324" s="18"/>
-      <c r="G324" s="55"/>
-      <c r="H324" s="55"/>
+      <c r="G324" s="55" t="s">
+        <v>1367</v>
+      </c>
+      <c r="H324" s="55" t="s">
+        <v>1368</v>
+      </c>
       <c r="I324" s="18"/>
       <c r="J324" s="18">
         <v>15435</v>
@@ -17137,7 +17138,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="325" spans="1:12" ht="57.6">
+    <row r="325" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A325" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17173,7 +17174,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="326" spans="1:12" ht="86.45">
+    <row r="326" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A326" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17209,7 +17210,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="327" spans="1:12" ht="72">
+    <row r="327" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A327" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17245,7 +17246,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="328" spans="1:12" ht="57.6">
+    <row r="328" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A328" s="18" t="s">
         <v>1328</v>
       </c>
@@ -17281,7 +17282,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="329" spans="1:12" ht="72">
+    <row r="329" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A329" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17319,7 +17320,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="330" spans="1:12" ht="72">
+    <row r="330" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A330" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17357,7 +17358,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="331" spans="1:12" ht="72">
+    <row r="331" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A331" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17395,7 +17396,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="332" spans="1:12" ht="158.44999999999999">
+    <row r="332" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A332" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17433,7 +17434,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="333" spans="1:12" ht="158.44999999999999">
+    <row r="333" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A333" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17471,7 +17472,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="334" spans="1:12" ht="158.44999999999999">
+    <row r="334" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A334" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17509,7 +17510,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="335" spans="1:12" ht="158.44999999999999">
+    <row r="335" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A335" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17547,7 +17548,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="336" spans="1:12" ht="158.44999999999999">
+    <row r="336" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A336" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17585,7 +17586,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="337" spans="1:12" ht="158.44999999999999">
+    <row r="337" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A337" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17623,7 +17624,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="338" spans="1:12" ht="158.44999999999999">
+    <row r="338" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A338" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17661,7 +17662,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="339" spans="1:12" ht="158.44999999999999">
+    <row r="339" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A339" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17699,7 +17700,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="340" spans="1:12" ht="100.9">
+    <row r="340" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A340" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17737,7 +17738,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="341" spans="1:12" ht="158.44999999999999">
+    <row r="341" spans="1:12" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A341" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17775,7 +17776,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="342" spans="1:12" ht="72">
+    <row r="342" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A342" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17813,7 +17814,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="343" spans="1:12" ht="72">
+    <row r="343" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A343" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17851,7 +17852,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="344" spans="1:12" ht="72">
+    <row r="344" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A344" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17889,7 +17890,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="345" spans="1:12" ht="72">
+    <row r="345" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A345" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17927,7 +17928,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="346" spans="1:12" ht="72">
+    <row r="346" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A346" s="19" t="s">
         <v>1399</v>
       </c>
@@ -17965,7 +17966,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="347" spans="1:12" ht="72">
+    <row r="347" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A347" s="19" t="s">
         <v>1399</v>
       </c>
@@ -18003,7 +18004,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="348" spans="1:12" ht="72">
+    <row r="348" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A348" s="19" t="s">
         <v>1399</v>
       </c>
@@ -18041,7 +18042,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="349" spans="1:12" ht="72">
+    <row r="349" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A349" s="19" t="s">
         <v>1399</v>
       </c>
@@ -18079,7 +18080,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="350" spans="1:12" ht="72">
+    <row r="350" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A350" s="19" t="s">
         <v>1399</v>
       </c>
@@ -18117,7 +18118,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="351" spans="1:12" ht="201.6">
+    <row r="351" spans="1:12" ht="204" x14ac:dyDescent="0.4">
       <c r="A351" s="19" t="s">
         <v>1399</v>
       </c>
@@ -18155,7 +18156,7 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="352" spans="1:12" ht="100.9">
+    <row r="352" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A352" s="44" t="s">
         <v>1399</v>
       </c>
@@ -18193,7 +18194,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="353" spans="1:13" ht="216">
+    <row r="353" spans="1:13" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A353" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18231,7 +18232,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="354" spans="1:13" ht="129.6">
+    <row r="354" spans="1:13" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A354" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18269,7 +18270,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="355" spans="1:13" ht="158.44999999999999">
+    <row r="355" spans="1:13" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A355" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18310,7 +18311,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="356" spans="1:13" ht="216">
+    <row r="356" spans="1:13" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A356" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18348,7 +18349,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="357" spans="1:13" ht="230.45">
+    <row r="357" spans="1:13" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A357" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18386,7 +18387,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="358" spans="1:13" ht="129.6">
+    <row r="358" spans="1:13" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A358" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18424,7 +18425,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="359" spans="1:13" ht="144">
+    <row r="359" spans="1:13" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A359" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18462,7 +18463,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="360" spans="1:13" ht="100.9">
+    <row r="360" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A360" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18500,7 +18501,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="361" spans="1:13" ht="158.44999999999999">
+    <row r="361" spans="1:13" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A361" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18538,7 +18539,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="362" spans="1:13" ht="115.15">
+    <row r="362" spans="1:13" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A362" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18573,7 +18574,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="363" spans="1:13" ht="144">
+    <row r="363" spans="1:13" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A363" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18592,7 +18593,7 @@
       <c r="F363" s="43">
         <v>38808</v>
       </c>
-      <c r="G363" s="106" t="s">
+      <c r="G363" s="105" t="s">
         <v>1138</v>
       </c>
       <c r="H363" s="59" t="s">
@@ -18608,7 +18609,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="364" spans="1:13" ht="43.15">
+    <row r="364" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A364" s="76" t="s">
         <v>1522</v>
       </c>
@@ -18640,7 +18641,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="365" spans="1:13" ht="172.9">
+    <row r="365" spans="1:13" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A365" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18678,7 +18679,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="366" spans="1:13" ht="158.44999999999999">
+    <row r="366" spans="1:13" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A366" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18716,7 +18717,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="367" spans="1:13" ht="115.15">
+    <row r="367" spans="1:13" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A367" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18754,7 +18755,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="368" spans="1:13" ht="158.44999999999999">
+    <row r="368" spans="1:13" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A368" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18792,7 +18793,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="369" spans="1:13" ht="129.6">
+    <row r="369" spans="1:13" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A369" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18830,7 +18831,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="370" spans="1:13" ht="115.15">
+    <row r="370" spans="1:13" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A370" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18868,7 +18869,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="371" spans="1:13" ht="100.9">
+    <row r="371" spans="1:13" ht="102" x14ac:dyDescent="0.4">
       <c r="A371" s="42" t="s">
         <v>1522</v>
       </c>
@@ -18906,7 +18907,7 @@
         <v>1618</v>
       </c>
     </row>
-    <row r="372" spans="1:13" ht="72">
+    <row r="372" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A372" s="77" t="s">
         <v>1522</v>
       </c>
@@ -18937,7 +18938,7 @@
         <v>1621</v>
       </c>
     </row>
-    <row r="373" spans="1:13" ht="187.15">
+    <row r="373" spans="1:13" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A373" s="36" t="s">
         <v>1522</v>
       </c>
@@ -18972,7 +18973,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="374" spans="1:13" ht="57.6">
+    <row r="374" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A374" s="76" t="s">
         <v>1522</v>
       </c>
@@ -18985,13 +18986,17 @@
       <c r="D374" s="80"/>
       <c r="E374" s="78"/>
       <c r="F374" s="77"/>
-      <c r="G374" s="99"/>
-      <c r="H374" s="81"/>
+      <c r="G374" s="58" t="s">
+        <v>255</v>
+      </c>
+      <c r="H374" s="59" t="s">
+        <v>1327</v>
+      </c>
       <c r="I374" s="80"/>
       <c r="J374" s="80"/>
       <c r="K374" s="76"/>
     </row>
-    <row r="375" spans="1:13" ht="86.45">
+    <row r="375" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A375" s="36" t="s">
         <v>1629</v>
       </c>
@@ -19008,7 +19013,7 @@
       <c r="F375" s="36">
         <v>2010</v>
       </c>
-      <c r="G375" s="100" t="s">
+      <c r="G375" s="99" t="s">
         <v>1413</v>
       </c>
       <c r="H375" s="58" t="s">
@@ -19045,26 +19050,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cdd28b36-9559-4f02-b334-18686e08c090">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="edb9d0e4-5370-4cfb-9e4e-bdf6de379f60" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100362CCE852358CD488E8AC7D76A88A7B9" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0a969f11f333e55a635863768f56c1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cdd28b36-9559-4f02-b334-18686e08c090" xmlns:ns3="96b41f5b-68c8-47b0-939c-7829c37ecb01" xmlns:ns4="edb9d0e4-5370-4cfb-9e4e-bdf6de379f60" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8b960cfa97ac6e5019242c462d73d63" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="cdd28b36-9559-4f02-b334-18686e08c090"/>
@@ -19324,14 +19309,61 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cdd28b36-9559-4f02-b334-18686e08c090">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="edb9d0e4-5370-4cfb-9e4e-bdf6de379f60" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B63753ED-2BDE-41D8-AA6D-C8D4B1838EF9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E6439D9-5C72-4491-BBC5-0A456A97ACC6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cdd28b36-9559-4f02-b334-18686e08c090"/>
+    <ds:schemaRef ds:uri="96b41f5b-68c8-47b0-939c-7829c37ecb01"/>
+    <ds:schemaRef ds:uri="edb9d0e4-5370-4cfb-9e4e-bdf6de379f60"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECFE642C-065B-42D7-988C-837700AA9EA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECFE642C-065B-42D7-988C-837700AA9EA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E6439D9-5C72-4491-BBC5-0A456A97ACC6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B63753ED-2BDE-41D8-AA6D-C8D4B1838EF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cdd28b36-9559-4f02-b334-18686e08c090"/>
+    <ds:schemaRef ds:uri="edb9d0e4-5370-4cfb-9e4e-bdf6de379f60"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>